<commit_message>
hopefully got them all
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>CPU SEQ</t>
   </si>
@@ -44,10 +44,13 @@
     <t>RUNS</t>
   </si>
   <si>
-    <t>SIZE = 2000</t>
+    <t>SIZE = 6144</t>
   </si>
   <si>
-    <t>SIZE = 6144</t>
+    <t>SIZE = 2048</t>
+  </si>
+  <si>
+    <t>SIZE = 1000</t>
   </si>
 </sst>
 </file>
@@ -155,7 +158,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -173,7 +179,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="H3:L13" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="H3:L13" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="H3:L13">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -203,6 +209,26 @@
     <tableColumn id="1" name="RUNS"/>
     <tableColumn id="2" name="CPU SEQ"/>
     <tableColumn id="3" name="GPU SEQ"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="O3:S13" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="O3:S13">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" name="RUNS"/>
+    <tableColumn id="2" name="CPU SEQ"/>
+    <tableColumn id="3" name="GPU PARALLEL"/>
+    <tableColumn id="4" name="GPU ATOMIC"/>
+    <tableColumn id="6" name="GPU SHARED ATOMIC"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -471,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L13"/>
+  <dimension ref="B1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,24 +514,37 @@
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
     <col min="12" max="12" width="21.85546875" customWidth="1"/>
+    <col min="14" max="14" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
       <c r="H2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="5"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
@@ -532,14 +571,36 @@
       <c r="L3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N3" s="1"/>
+      <c r="O3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
+      <c r="D4">
+        <v>4.8550000000000004</v>
+      </c>
+      <c r="E4">
+        <v>12.221</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
@@ -549,12 +610,36 @@
       <c r="I4">
         <v>1214.6859999999999</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>40.289000000000001</v>
+      </c>
+      <c r="Q4">
+        <v>5.6260000000000003</v>
+      </c>
+      <c r="R4">
+        <v>3.1789999999999998</v>
+      </c>
+      <c r="S4">
+        <v>2.5409999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5">
         <v>2</v>
       </c>
+      <c r="D5">
+        <v>4.8559999999999999</v>
+      </c>
+      <c r="E5">
+        <v>12.586</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5">
         <v>2</v>
@@ -562,12 +647,34 @@
       <c r="I5">
         <v>1221.048</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N5" s="2"/>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>40.210999999999999</v>
+      </c>
+      <c r="Q5">
+        <v>5.6219999999999999</v>
+      </c>
+      <c r="R5">
+        <v>3.198</v>
+      </c>
+      <c r="S5">
+        <v>2.7290000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6">
         <v>3</v>
       </c>
+      <c r="D6">
+        <v>4.8609999999999998</v>
+      </c>
+      <c r="E6">
+        <v>14.233000000000001</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6">
         <v>3</v>
@@ -575,88 +682,261 @@
       <c r="I6">
         <v>1216.7850000000001</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N6" s="2"/>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>40.215000000000003</v>
+      </c>
+      <c r="Q6">
+        <v>5.6390000000000002</v>
+      </c>
+      <c r="R6">
+        <v>3.2069999999999999</v>
+      </c>
+      <c r="S6">
+        <v>2.7930000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7">
         <v>4</v>
       </c>
+      <c r="D7">
+        <v>5.1050000000000004</v>
+      </c>
+      <c r="E7">
+        <v>11.688000000000001</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N7" s="2"/>
+      <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <v>40.222000000000001</v>
+      </c>
+      <c r="Q7">
+        <v>5.625</v>
+      </c>
+      <c r="R7">
+        <v>3.2290000000000001</v>
+      </c>
+      <c r="S7">
+        <v>2.819</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8">
         <v>5</v>
       </c>
+      <c r="D8">
+        <v>4.8540000000000001</v>
+      </c>
+      <c r="E8">
+        <v>10.478</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N8" s="2"/>
+      <c r="O8">
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <v>40.219000000000001</v>
+      </c>
+      <c r="Q8">
+        <v>5.6139999999999999</v>
+      </c>
+      <c r="R8">
+        <v>3.226</v>
+      </c>
+      <c r="S8">
+        <v>2.7490000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9">
         <v>6</v>
       </c>
+      <c r="D9">
+        <v>4.8570000000000002</v>
+      </c>
+      <c r="E9">
+        <v>11.461</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N9" s="2"/>
+      <c r="O9">
+        <v>6</v>
+      </c>
+      <c r="P9">
+        <v>40.889000000000003</v>
+      </c>
+      <c r="Q9">
+        <v>5.617</v>
+      </c>
+      <c r="R9">
+        <v>3.2050000000000001</v>
+      </c>
+      <c r="S9">
+        <v>2.7519999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10">
         <v>7</v>
       </c>
+      <c r="D10">
+        <v>4.8550000000000004</v>
+      </c>
+      <c r="E10">
+        <v>12.319000000000001</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N10" s="2"/>
+      <c r="O10">
+        <v>7</v>
+      </c>
+      <c r="P10">
+        <v>40.892000000000003</v>
+      </c>
+      <c r="Q10">
+        <v>5.6130000000000004</v>
+      </c>
+      <c r="R10">
+        <v>3.2309999999999999</v>
+      </c>
+      <c r="S10">
+        <v>2.5489999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11">
         <v>8</v>
       </c>
+      <c r="D11">
+        <v>4.8550000000000004</v>
+      </c>
+      <c r="E11">
+        <v>10.576000000000001</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N11" s="2"/>
+      <c r="O11">
+        <v>8</v>
+      </c>
+      <c r="P11">
+        <v>40.198999999999998</v>
+      </c>
+      <c r="Q11">
+        <v>5.6269999999999998</v>
+      </c>
+      <c r="R11">
+        <v>3.2050000000000001</v>
+      </c>
+      <c r="S11">
+        <v>2.5430000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12">
         <v>9</v>
       </c>
+      <c r="D12">
+        <v>4.8540000000000001</v>
+      </c>
+      <c r="E12">
+        <v>12.923999999999999</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N12" s="2"/>
+      <c r="O12">
+        <v>9</v>
+      </c>
+      <c r="P12">
+        <v>40.220999999999997</v>
+      </c>
+      <c r="Q12">
+        <v>5.649</v>
+      </c>
+      <c r="R12">
+        <v>3.2069999999999999</v>
+      </c>
+      <c r="S12">
+        <v>2.5510000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13">
         <v>10</v>
       </c>
+      <c r="D13">
+        <v>4.8550000000000004</v>
+      </c>
+      <c r="E13">
+        <v>11.552</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13">
         <v>10</v>
       </c>
+      <c r="N13" s="2"/>
+      <c r="O13">
+        <v>10</v>
+      </c>
+      <c r="P13">
+        <v>40.223999999999997</v>
+      </c>
+      <c r="Q13">
+        <v>5.617</v>
+      </c>
+      <c r="R13">
+        <v>3.1589999999999998</v>
+      </c>
+      <c r="S13">
+        <v>2.7309999999999999</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="G4:G13"/>
     <mergeCell ref="B4:B13"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="C2:E2"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="N4:N13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>